<commit_message>
ControllerTables correct now probably
</commit_message>
<xml_diff>
--- a/ControllerTables.xlsx
+++ b/ControllerTables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t xml:space="preserve">State transition</t>
   </si>
@@ -52,40 +52,46 @@
     <t xml:space="preserve">A+</t>
   </si>
   <si>
+    <t xml:space="preserve">Z2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z0</t>
+  </si>
+  <si>
     <t xml:space="preserve">T8</t>
   </si>
   <si>
     <t xml:space="preserve">T4</t>
   </si>
   <si>
-    <t xml:space="preserve">Assuming done is 1 rather than x</t>
-  </si>
-  <si>
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">C+ = C’BAD + CB’A’ + CBD + CA’D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B+ = B’AD + BA’D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A+ = A’D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z = CB’A’ + CD ???</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Y = BD                ???</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X = AD               ???</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T8 = C’B’A’D’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T4 = CB’A’D’</t>
+    <t xml:space="preserve">C+ = CB’ + CA’ + C’BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B+ = B’A + BA’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A+ = BA’ + CA’done +A’donesensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2 = C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z1 = B               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z0 = A               </t>
+  </si>
+  <si>
+    <t xml:space="preserve">T8 = CBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T4 = C’BA</t>
   </si>
 </sst>
 </file>
@@ -301,7 +307,7 @@
   <dimension ref="A2:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4:O15"/>
+      <selection pane="topLeft" activeCell="R24" activeCellId="0" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -346,22 +352,19 @@
         <v>9</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,7 +384,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>0</v>
@@ -487,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="4" t="n">
         <v>0</v>
@@ -510,10 +513,10 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>0</v>
@@ -554,10 +557,10 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>0</v>
@@ -598,10 +601,10 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>1</v>
@@ -645,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>1</v>
@@ -689,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H12" s="0" t="n">
         <v>1</v>
@@ -730,10 +733,10 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>1</v>
@@ -760,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -777,10 +780,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H14" s="0" t="n">
         <v>1</v>
@@ -807,7 +810,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -824,10 +827,10 @@
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>0</v>
@@ -854,33 +857,33 @@
         <v>0</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T17" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T18" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T19" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T21" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T22" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>